<commit_message>
Added C1 user stories
</commit_message>
<xml_diff>
--- a/User Stories [TEMPLATE].xlsx
+++ b/User Stories [TEMPLATE].xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DINA\Desktop\T17-Sprint2\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{D996DB62-ECD1-43C1-904B-E664E41E3B76}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories" sheetId="1" r:id="rId1"/>
     <sheet name="Analysis" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" iterateDelta="1E-4"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -20,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t xml:space="preserve"> EPIC</t>
   </si>
@@ -80,6 +86,9 @@
   </si>
   <si>
     <t>1 High</t>
+  </si>
+  <si>
+    <t>LG</t>
   </si>
   <si>
     <t>[A list of acceptance tests]</t>
@@ -174,47 +183,11 @@
   <si>
     <t>Verify that the user can search by expert name and  that the returned results are complete and correct.</t>
   </si>
-  <si>
-    <t>As an expert , I can add a topic</t>
-  </si>
-  <si>
-    <t>As a user, I can apply to be an expert</t>
-  </si>
-  <si>
-    <t>As an admin , I can accept or reject experts applications</t>
-  </si>
-  <si>
-    <t>the user get notification that the application is done and the admins can see this application</t>
-  </si>
-  <si>
-    <t>in case if acceptance the user become an expert and in case of rejection the user get notifiication that his application rejected</t>
-  </si>
-  <si>
-    <t>the topic added in the list of the expert's topics</t>
-  </si>
-  <si>
-    <t>SM</t>
-  </si>
-  <si>
-    <t>MD</t>
-  </si>
-  <si>
-    <t>XSM</t>
-  </si>
-  <si>
-    <t>2 Med</t>
-  </si>
-  <si>
-    <t>4 Low</t>
-  </si>
-  <si>
-    <t>3 Med</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7">
     <font>
       <sz val="10"/>
@@ -343,7 +316,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -413,15 +386,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1025,14 +989,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF3C78D8"/>
   </sheetPr>
@@ -1040,7 +1004,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1116,27 +1080,31 @@
     <row r="2" spans="1:19" ht="22.5">
       <c r="A2" s="9"/>
       <c r="B2" s="10"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="12"/>
+      <c r="C2" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>20</v>
+      </c>
       <c r="E2" s="24" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G2" s="24" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I2" s="15" t="e">
         <f>IF(AND(OR(#REF!="1 High",#REF!="2 Med"),OR(#REF!="1 High",#REF!="2 Med")),"Strategic",IF(AND(OR(#REF!="1 High",#REF!="2 Med"),OR(#REF!="3 Med",#REF!="4 Low")),"Leveraged",IF(AND(OR(#REF!="3 Med",#REF!="4 Low"),OR(#REF!="1 High",#REF!="2 Med")),"Focused",IF(AND(OR(#REF!="3 Med",#REF!="4 Low"),OR(#REF!="3 Med",#REF!="4 Low")),"Routine",""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="J2" s="16" t="str">
+      <c r="J2" s="16">
         <f t="shared" ref="J2:J65" si="0">IF(C2="1 High",1,IF(C2="2 Med",2,IF(C2="3 Med",3,IF(C2="4 Low",4,""))))</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="K2" s="17" t="e">
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
@@ -1146,9 +1114,9 @@
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="M2" s="16" t="str">
+      <c r="M2" s="16">
         <f t="shared" ref="M2:M65" si="1">IF(C2="1 High",4,IF(C2="2 Med",3,IF(C2="3 Med",2,IF(C2="4 Low",1,""))))</f>
-        <v/>
+        <v>4</v>
       </c>
       <c r="N2" s="16" t="e">
         <f>IF(#REF!="1 High",4,IF(#REF!="2 Med",3,IF(#REF!="3 Med",2,IF(#REF!="4 Low",1,""))))</f>
@@ -1163,7 +1131,7 @@
         <v>[Theme, Epic, or Dept]</v>
       </c>
       <c r="Q2" s="18" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="R2" s="19" t="e">
         <f>IF(#REF!="MVP","0.0 MVP",#REF!)</f>
@@ -1176,27 +1144,23 @@
     </row>
     <row r="3" spans="1:19" ht="45">
       <c r="A3" s="21" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="D3" s="29" t="s">
-        <v>58</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="12"/>
       <c r="E3" s="25" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
       <c r="H3" s="14"/>
       <c r="I3" s="15"/>
-      <c r="J3" s="16">
+      <c r="J3" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v/>
       </c>
       <c r="K3" s="17" t="e">
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
@@ -1206,9 +1170,9 @@
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="M3" s="16">
+      <c r="M3" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v/>
       </c>
       <c r="N3" s="16" t="e">
         <f>IF(#REF!="1 High",4,IF(#REF!="2 Med",3,IF(#REF!="3 Med",2,IF(#REF!="4 Low",1,""))))</f>
@@ -1235,24 +1199,20 @@
     <row r="4" spans="1:19" ht="33.75">
       <c r="A4" s="9"/>
       <c r="B4" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" s="29" t="s">
-        <v>58</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="C4" s="11"/>
+      <c r="D4" s="12"/>
       <c r="E4" s="25" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
       <c r="H4" s="14"/>
       <c r="I4" s="15"/>
-      <c r="J4" s="16">
+      <c r="J4" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v/>
       </c>
       <c r="K4" s="17" t="e">
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
@@ -1262,9 +1222,9 @@
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="M4" s="16">
+      <c r="M4" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v/>
       </c>
       <c r="N4" s="16" t="e">
         <f>IF(#REF!="1 High",4,IF(#REF!="2 Med",3,IF(#REF!="3 Med",2,IF(#REF!="4 Low",1,""))))</f>
@@ -1291,24 +1251,20 @@
     <row r="5" spans="1:19" ht="45">
       <c r="A5" s="9"/>
       <c r="B5" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" s="29" t="s">
-        <v>58</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="C5" s="11"/>
+      <c r="D5" s="12"/>
       <c r="E5" s="25" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
       <c r="H5" s="14"/>
       <c r="I5" s="15"/>
-      <c r="J5" s="16">
+      <c r="J5" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v/>
       </c>
       <c r="K5" s="17" t="e">
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
@@ -1318,9 +1274,9 @@
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="M5" s="16">
+      <c r="M5" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v/>
       </c>
       <c r="N5" s="16" t="e">
         <f>IF(#REF!="1 High",4,IF(#REF!="2 Med",3,IF(#REF!="3 Med",2,IF(#REF!="4 Low",1,""))))</f>
@@ -1346,25 +1302,21 @@
     </row>
     <row r="6" spans="1:19" ht="45">
       <c r="A6" s="9"/>
-      <c r="B6" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="29" t="s">
-        <v>58</v>
-      </c>
+      <c r="B6" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="11"/>
+      <c r="D6" s="12"/>
       <c r="E6" s="13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
       <c r="H6" s="14"/>
       <c r="I6" s="15"/>
-      <c r="J6" s="16">
+      <c r="J6" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="K6" s="17" t="e">
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
@@ -1374,9 +1326,9 @@
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="M6" s="16">
+      <c r="M6" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v/>
       </c>
       <c r="N6" s="16" t="e">
         <f>IF(#REF!="1 High",4,IF(#REF!="2 Med",3,IF(#REF!="3 Med",2,IF(#REF!="4 Low",1,""))))</f>
@@ -1402,25 +1354,21 @@
     </row>
     <row r="7" spans="1:19" ht="33.75">
       <c r="A7" s="9"/>
-      <c r="B7" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="29" t="s">
-        <v>57</v>
-      </c>
+      <c r="B7" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="11"/>
+      <c r="D7" s="12"/>
       <c r="E7" s="13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
       <c r="H7" s="14"/>
       <c r="I7" s="15"/>
-      <c r="J7" s="16">
+      <c r="J7" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="K7" s="17" t="e">
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
@@ -1430,9 +1378,9 @@
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="M7" s="16">
+      <c r="M7" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v/>
       </c>
       <c r="N7" s="16" t="e">
         <f>IF(#REF!="1 High",4,IF(#REF!="2 Med",3,IF(#REF!="3 Med",2,IF(#REF!="4 Low",1,""))))</f>
@@ -1698,27 +1646,23 @@
     </row>
     <row r="13" spans="1:19" ht="33.75">
       <c r="A13" s="23" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="29" t="s">
-        <v>59</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="C13" s="11"/>
+      <c r="D13" s="12"/>
       <c r="E13" s="25" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
       <c r="H13" s="14"/>
       <c r="I13" s="15"/>
-      <c r="J13" s="16">
+      <c r="J13" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="K13" s="17" t="e">
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
@@ -1728,9 +1672,9 @@
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="M13" s="16">
+      <c r="M13" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v/>
       </c>
       <c r="N13" s="16" t="e">
         <f>IF(#REF!="1 High",4,IF(#REF!="2 Med",3,IF(#REF!="3 Med",2,IF(#REF!="4 Low",1,""))))</f>
@@ -1757,24 +1701,20 @@
     <row r="14" spans="1:19" ht="56.25">
       <c r="A14" s="9"/>
       <c r="B14" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="29" t="s">
-        <v>58</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="12"/>
       <c r="E14" s="25" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
       <c r="H14" s="14"/>
       <c r="I14" s="15"/>
-      <c r="J14" s="16">
+      <c r="J14" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="K14" s="17" t="e">
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
@@ -1784,9 +1724,9 @@
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="M14" s="16">
+      <c r="M14" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v/>
       </c>
       <c r="N14" s="16" t="e">
         <f>IF(#REF!="1 High",4,IF(#REF!="2 Med",3,IF(#REF!="3 Med",2,IF(#REF!="4 Low",1,""))))</f>
@@ -1813,24 +1753,20 @@
     <row r="15" spans="1:19" ht="45">
       <c r="A15" s="9"/>
       <c r="B15" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="D15" s="29" t="s">
-        <v>57</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="C15" s="11"/>
+      <c r="D15" s="12"/>
       <c r="E15" s="25" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F15" s="13"/>
       <c r="G15" s="13"/>
       <c r="H15" s="14"/>
       <c r="I15" s="15"/>
-      <c r="J15" s="16">
+      <c r="J15" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v/>
       </c>
       <c r="K15" s="17" t="e">
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
@@ -1840,9 +1776,9 @@
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="M15" s="16">
+      <c r="M15" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="N15" s="16" t="e">
         <f>IF(#REF!="1 High",4,IF(#REF!="2 Med",3,IF(#REF!="3 Med",2,IF(#REF!="4 Low",1,""))))</f>
@@ -1917,24 +1853,20 @@
     <row r="17" spans="1:19" ht="33.75">
       <c r="A17" s="9"/>
       <c r="B17" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="D17" s="29" t="s">
-        <v>57</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="C17" s="11"/>
+      <c r="D17" s="12"/>
       <c r="E17" s="25" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F17" s="13"/>
       <c r="G17" s="13"/>
       <c r="H17" s="14"/>
       <c r="I17" s="15"/>
-      <c r="J17" s="16">
+      <c r="J17" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v/>
       </c>
       <c r="K17" s="17" t="e">
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
@@ -1944,9 +1876,9 @@
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="M17" s="16">
+      <c r="M17" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v/>
       </c>
       <c r="N17" s="16" t="e">
         <f>IF(#REF!="1 High",4,IF(#REF!="2 Med",3,IF(#REF!="3 Med",2,IF(#REF!="4 Low",1,""))))</f>
@@ -2021,24 +1953,20 @@
     <row r="19" spans="1:19" ht="56.25">
       <c r="A19" s="9"/>
       <c r="B19" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="C19" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="D19" s="29" t="s">
-        <v>57</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="C19" s="11"/>
+      <c r="D19" s="12"/>
       <c r="E19" s="25" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F19" s="13"/>
       <c r="G19" s="13"/>
       <c r="H19" s="14"/>
       <c r="I19" s="15"/>
-      <c r="J19" s="16">
+      <c r="J19" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v/>
       </c>
       <c r="K19" s="17" t="e">
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
@@ -2048,9 +1976,9 @@
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="M19" s="16">
+      <c r="M19" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v/>
       </c>
       <c r="N19" s="16" t="e">
         <f>IF(#REF!="1 High",4,IF(#REF!="2 Med",3,IF(#REF!="3 Med",2,IF(#REF!="4 Low",1,""))))</f>
@@ -2124,25 +2052,21 @@
     </row>
     <row r="21" spans="1:19" ht="33.75">
       <c r="A21" s="9"/>
-      <c r="B21" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="C21" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="D21" s="29" t="s">
-        <v>57</v>
-      </c>
+      <c r="B21" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="11"/>
+      <c r="D21" s="12"/>
       <c r="E21" s="13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F21" s="13"/>
       <c r="G21" s="13"/>
       <c r="H21" s="14"/>
       <c r="I21" s="15"/>
-      <c r="J21" s="16">
+      <c r="J21" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v/>
       </c>
       <c r="K21" s="17" t="e">
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
@@ -2152,9 +2076,9 @@
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="M21" s="16">
+      <c r="M21" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v/>
       </c>
       <c r="N21" s="16" t="e">
         <f>IF(#REF!="1 High",4,IF(#REF!="2 Med",3,IF(#REF!="3 Med",2,IF(#REF!="4 Low",1,""))))</f>
@@ -2180,25 +2104,21 @@
     </row>
     <row r="22" spans="1:19" ht="33.75">
       <c r="A22" s="9"/>
-      <c r="B22" s="22" t="s">
+      <c r="B22" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="11"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="13" t="s">
         <v>46</v>
-      </c>
-      <c r="C22" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="D22" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>45</v>
       </c>
       <c r="F22" s="13"/>
       <c r="G22" s="13"/>
       <c r="H22" s="14"/>
       <c r="I22" s="15"/>
-      <c r="J22" s="16">
+      <c r="J22" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="K22" s="17" t="e">
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
@@ -2208,9 +2128,9 @@
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="M22" s="16">
+      <c r="M22" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v/>
       </c>
       <c r="N22" s="16" t="e">
         <f>IF(#REF!="1 High",4,IF(#REF!="2 Med",3,IF(#REF!="3 Med",2,IF(#REF!="4 Low",1,""))))</f>
@@ -2236,7 +2156,7 @@
     </row>
     <row r="23" spans="1:19">
       <c r="A23" s="9"/>
-      <c r="B23" s="22"/>
+      <c r="B23" s="10"/>
       <c r="C23" s="11"/>
       <c r="D23" s="12"/>
       <c r="E23" s="13"/>
@@ -2330,27 +2250,19 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="22.5">
+    <row r="25" spans="1:19">
       <c r="A25" s="9"/>
-      <c r="B25" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="C25" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="E25" s="13" t="s">
-        <v>56</v>
-      </c>
+      <c r="B25" s="10"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="13"/>
       <c r="F25" s="13"/>
       <c r="G25" s="13"/>
       <c r="H25" s="14"/>
       <c r="I25" s="15"/>
-      <c r="J25" s="16">
+      <c r="J25" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="K25" s="17" t="e">
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
@@ -2360,9 +2272,9 @@
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="M25" s="16">
+      <c r="M25" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v/>
       </c>
       <c r="N25" s="16" t="e">
         <f>IF(#REF!="1 High",4,IF(#REF!="2 Med",3,IF(#REF!="3 Med",2,IF(#REF!="4 Low",1,""))))</f>
@@ -2381,9 +2293,9 @@
         <f>IF(#REF!="MVP","0.0 MVP",#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="S25" s="20">
+      <c r="S25" s="20" t="str">
         <f t="shared" si="2"/>
-        <v>25</v>
+        <v/>
       </c>
     </row>
     <row r="26" spans="1:19">
@@ -2434,27 +2346,19 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="33.75">
+    <row r="27" spans="1:19">
       <c r="A27" s="9"/>
-      <c r="B27" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="C27" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="E27" s="13" t="s">
-        <v>54</v>
-      </c>
+      <c r="B27" s="10"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="13"/>
       <c r="F27" s="13"/>
       <c r="G27" s="13"/>
       <c r="H27" s="14"/>
       <c r="I27" s="15"/>
-      <c r="J27" s="16">
+      <c r="J27" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="K27" s="17" t="e">
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
@@ -2464,9 +2368,9 @@
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="M27" s="16">
+      <c r="M27" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v/>
       </c>
       <c r="N27" s="16" t="e">
         <f>IF(#REF!="1 High",4,IF(#REF!="2 Med",3,IF(#REF!="3 Med",2,IF(#REF!="4 Low",1,""))))</f>
@@ -2485,9 +2389,9 @@
         <f>IF(#REF!="MVP","0.0 MVP",#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="S27" s="20">
+      <c r="S27" s="20" t="str">
         <f t="shared" si="2"/>
-        <v>27</v>
+        <v/>
       </c>
     </row>
     <row r="28" spans="1:19">
@@ -2538,27 +2442,19 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="45">
+    <row r="29" spans="1:19">
       <c r="A29" s="9"/>
-      <c r="B29" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="C29" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="D29" s="29" t="s">
-        <v>58</v>
-      </c>
-      <c r="E29" s="13" t="s">
-        <v>55</v>
-      </c>
+      <c r="B29" s="10"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="13"/>
       <c r="F29" s="13"/>
       <c r="G29" s="13"/>
       <c r="H29" s="14"/>
       <c r="I29" s="15"/>
-      <c r="J29" s="16">
+      <c r="J29" s="16" t="str">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="K29" s="17" t="e">
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
@@ -2568,9 +2464,9 @@
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="M29" s="16">
+      <c r="M29" s="16" t="str">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v/>
       </c>
       <c r="N29" s="16" t="e">
         <f>IF(#REF!="1 High",4,IF(#REF!="2 Med",3,IF(#REF!="3 Med",2,IF(#REF!="4 Low",1,""))))</f>
@@ -2589,9 +2485,9 @@
         <f>IF(#REF!="MVP","0.0 MVP",#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="S29" s="20">
+      <c r="S29" s="20" t="str">
         <f t="shared" si="2"/>
-        <v>29</v>
+        <v/>
       </c>
     </row>
     <row r="30" spans="1:19">
@@ -51756,11 +51652,11 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" sqref="C2:C1000">
+    <dataValidation type="list" allowBlank="1" sqref="C2:C1000" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"1 High,2 Med,3 Med,4 Low"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D2:D1000">
+    <dataValidation type="list" allowBlank="1" sqref="D2:D1000" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"XSM,SM,MD,LG,XLG,XXLG,0,0.5,1,2,3,5,8,13,21,34,55,89,?"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -51771,7 +51667,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FFA64D79"/>
   </sheetPr>

</xml_diff>

<commit_message>
adding c3 user stories
</commit_message>
<xml_diff>
--- a/User Stories [TEMPLATE].xlsx
+++ b/User Stories [TEMPLATE].xlsx
@@ -1,27 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DINA\Desktop\T17-Sprint2\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{54DECCAB-BF93-4F30-9770-596EC9372E5D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993"/>
   </bookViews>
   <sheets>
     <sheet name="User Stories" sheetId="1" r:id="rId1"/>
     <sheet name="Analysis" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="145621" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="185">
   <si>
     <t xml:space="preserve"> EPIC</t>
   </si>
@@ -457,11 +451,145 @@
   <si>
     <t xml:space="preserve">after hitting send the admin recieves a pop up message of the log of sent messages </t>
   </si>
+  <si>
+    <t>Manage Reservation</t>
+  </si>
+  <si>
+    <t>As a user I should be able to cancel a reservation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.A pop-up message will appear to confirm the cancellation
+2.The slot will be removed from the user and the expert shecdule
+</t>
+  </si>
+  <si>
+    <t>As an expert, I should be able to cancel a reserved session</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.A pop-up message will appear to confirm the cancellation
+2.The slot will be removed from the expert and the user shecdule
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a user  I want to be notified about any cancelled reservation. </t>
+  </si>
+  <si>
+    <t>1.A notification will be sent on the email and profile of the user</t>
+  </si>
+  <si>
+    <t>As an expert  I should be notified when a user changes any detail of a reserved slot</t>
+  </si>
+  <si>
+    <t>1.A notification will be sent on the email and profile of the expert</t>
+  </si>
+  <si>
+    <t>As an expert, I should be sent a notification if a user requested a cancellation</t>
+  </si>
+  <si>
+    <t>As a user I can view my reserved sessions</t>
+  </si>
+  <si>
+    <t>1.The user will be directed to his/her schedule</t>
+  </si>
+  <si>
+    <t>As a user I can reschedule a reservation timing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1.The expert will receive a notification on the email and profile
+2.The user will be sent new 3 slots to choose from </t>
+  </si>
+  <si>
+    <t>As an expert I can reschedule a reservation timing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1.The user will be sent 3 new slots to choose from or he/she can cancel the session
+3.If the user picked another slot the schedule of both the expert and the user will be updated</t>
+  </si>
+  <si>
+    <t>As a user I can change the communication method</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.A pop-up message will appear with the new session's info for the user to confirm
+2.A notification will be sent on the email and profile of the expert
+3.The schedule of the user and the expert will be updated </t>
+  </si>
+  <si>
+    <t>As an expert, I should be able to view all reserved slot'sinfo</t>
+  </si>
+  <si>
+    <t>1.The expert will be directed to his/her schedule</t>
+  </si>
+  <si>
+    <t>As a  user I can view other participantes in the group session</t>
+  </si>
+  <si>
+    <t>1.A list will appear with the participants usernames 
+2.The user will be redirected to any participant's profile upon clicking on his/her username</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a user I should be able to change the status of a reserved slot </t>
+  </si>
+  <si>
+    <t>As an expert, I should be able to block users, so they can't book reservations with me</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-A pop-up message will appear to ensure that the expert wants to block this certain user
+2.If the expert was in the user's favourite list he/she will be removed 
+3.The user will not be able to view the expert's profile
+4.The user will not get any results in the search about the expert </t>
+  </si>
+  <si>
+    <t>Favorite Experts</t>
+  </si>
+  <si>
+    <t>• As a user, I want to be able to add experts.</t>
+  </si>
+  <si>
+    <t>1-A pop-up message will appear to confirm that the experts has been added in the favorite experts</t>
+  </si>
+  <si>
+    <t>2- The user will find in the favorite experts the experts that he has choosen</t>
+  </si>
+  <si>
+    <t>• As a user, I want to be able to remove experts.</t>
+  </si>
+  <si>
+    <t>1-A pop-up message will appear to confirm that the experts has been removed in the favorite experts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2- The user will find in the favorite experts that the expert has been removed </t>
+  </si>
+  <si>
+    <t>• As a user, I want to be able to book a session with an expert</t>
+  </si>
+  <si>
+    <t>1.a pop-up message will appear to confirm the reservation</t>
+  </si>
+  <si>
+    <t>• As a user, I want to be able to search through the experts in my favorite experts.</t>
+  </si>
+  <si>
+    <t>1- The name of the expert appears when the user search for it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• As a user, I want to be able to add notes to each expert </t>
+  </si>
+  <si>
+    <t>1.The added note will appear beside the expert's name in the list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• As a user, I want to be able to navigate to each expert's profile page </t>
+  </si>
+  <si>
+    <t>1.The user will be directed to the expert profile page upon clicking on the expert's name</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="16">
     <font>
       <sz val="10"/>
@@ -813,9 +941,1371 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="46">
+  <dxfs count="184">
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF390C24"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF390C24"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7A1C4A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7A1C4A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFAD507E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFAD507E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCEA0B6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCEA0B6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEDB8D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEDB8D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF1E3E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF1E3E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF390C24"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF390C24"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF541235"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF541235"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7A1C4A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7A1C4A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9B4770"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9B4770"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFAD507E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFAD507E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCA80A6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCA80A6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCEA0B6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCEA0B6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDCAAC6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDCAAC6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEDB8D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEDB8D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF3D9E4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF3D9E4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF1E3E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF1E3E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF7E9EF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF7E9EF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEAEFF8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEAEFF8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF666666"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC9DAF8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF666666"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC9DAF8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA4C2F4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA4C2F4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF6D9EEB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF6D9EEB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF390C24"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF390C24"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7A1C4A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7A1C4A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFAD507E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFAD507E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCEA0B6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCEA0B6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEDB8D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEDB8D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF1E3E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF1E3E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF390C24"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF390C24"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF541235"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF541235"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7A1C4A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7A1C4A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9B4770"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9B4770"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFAD507E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFAD507E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCA80A6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCA80A6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCEA0B6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCEA0B6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDCAAC6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDCAAC6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEDB8D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEDB8D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF3D9E4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF3D9E4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF1E3E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF1E3E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF7E9EF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF7E9EF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEAEFF8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEAEFF8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF666666"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC9DAF8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF666666"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC9DAF8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA4C2F4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA4C2F4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF6D9EEB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF6D9EEB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF390C24"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF390C24"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7A1C4A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7A1C4A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFAD507E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFAD507E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCEA0B6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCEA0B6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEDB8D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEDB8D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF1E3E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF1E3E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF390C24"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF390C24"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF541235"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF541235"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7A1C4A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7A1C4A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9B4770"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9B4770"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFAD507E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFAD507E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCA80A6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCA80A6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCEA0B6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCEA0B6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDCAAC6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDCAAC6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEDB8D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEDB8D2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF3D9E4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF3D9E4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF1E3E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF1E3E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF7E9EF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF434343"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF7E9EF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCC0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEAEFF8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEAEFF8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF666666"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC9DAF8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF666666"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC9DAF8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA4C2F4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA4C2F4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF6D9EEB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF6D9EEB"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFFFFFF"/>
@@ -1663,22 +3153,22 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF3C78D8"/>
   </sheetPr>
   <dimension ref="A1:S1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F64" sqref="F64"/>
+      <pane ySplit="1" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A89" sqref="A89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -5278,7 +6768,7 @@
         <v/>
       </c>
     </row>
-    <row r="70" spans="1:19">
+    <row r="70" spans="1:19" ht="22.5">
       <c r="A70" s="9"/>
       <c r="B70" s="10" t="s">
         <v>129</v>
@@ -5334,7 +6824,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="71" spans="1:19">
+    <row r="71" spans="1:19" ht="22.5">
       <c r="A71" s="9"/>
       <c r="B71" s="10" t="s">
         <v>131</v>
@@ -5390,7 +6880,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="72" spans="1:19">
+    <row r="72" spans="1:19" ht="33.75">
       <c r="A72" s="9"/>
       <c r="B72" s="10" t="s">
         <v>133</v>
@@ -5550,7 +7040,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="75" spans="1:19">
+    <row r="75" spans="1:19" ht="33.75">
       <c r="A75" s="9"/>
       <c r="B75" s="10" t="s">
         <v>137</v>
@@ -5702,7 +7192,7 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="1:19">
+    <row r="78" spans="1:19" ht="33.75">
       <c r="A78" s="9"/>
       <c r="B78" s="10" t="s">
         <v>139</v>
@@ -5862,7 +7352,7 @@
         <v/>
       </c>
     </row>
-    <row r="81" spans="1:19">
+    <row r="81" spans="1:19" ht="33.75">
       <c r="A81" s="9"/>
       <c r="B81" s="10" t="s">
         <v>143</v>
@@ -6014,19 +7504,31 @@
         <v/>
       </c>
     </row>
-    <row r="84" spans="1:19">
-      <c r="A84" s="9"/>
-      <c r="B84" s="10"/>
-      <c r="C84" s="11"/>
-      <c r="D84" s="12"/>
-      <c r="E84" s="13"/>
-      <c r="F84" s="13"/>
+    <row r="84" spans="1:19" ht="56.25">
+      <c r="A84" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="B84" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="C84" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D84" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E84" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="F84" s="13" t="s">
+        <v>21</v>
+      </c>
       <c r="G84" s="13"/>
       <c r="H84" s="13"/>
       <c r="I84" s="15"/>
-      <c r="J84" s="16" t="str">
+      <c r="J84" s="16">
         <f t="shared" si="3"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="K84" s="17" t="e">
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
@@ -6036,9 +7538,9 @@
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="M84" s="16" t="str">
+      <c r="M84" s="16">
         <f t="shared" si="4"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="N84" s="16" t="e">
         <f>IF(#REF!="1 High",4,IF(#REF!="2 Med",3,IF(#REF!="3 Med",2,IF(#REF!="4 Low",1,""))))</f>
@@ -6057,24 +7559,34 @@
         <f>IF(#REF!="MVP","0.0 MVP",#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="S84" s="20" t="str">
+      <c r="S84" s="20">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="85" spans="1:19">
-      <c r="A85" s="9"/>
-      <c r="B85" s="10"/>
-      <c r="C85" s="11"/>
-      <c r="D85" s="12"/>
-      <c r="E85" s="13"/>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="85" spans="1:19" ht="56.25">
+      <c r="A85" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="B85" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="C85" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D85" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E85" s="13" t="s">
+        <v>149</v>
+      </c>
       <c r="F85" s="13"/>
       <c r="G85" s="13"/>
       <c r="H85" s="13"/>
       <c r="I85" s="15"/>
-      <c r="J85" s="16" t="str">
+      <c r="J85" s="16">
         <f t="shared" si="3"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="K85" s="17" t="e">
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
@@ -6084,9 +7596,9 @@
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="M85" s="16" t="str">
+      <c r="M85" s="16">
         <f t="shared" si="4"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="N85" s="16" t="e">
         <f>IF(#REF!="1 High",4,IF(#REF!="2 Med",3,IF(#REF!="3 Med",2,IF(#REF!="4 Low",1,""))))</f>
@@ -6105,9 +7617,9 @@
         <f>IF(#REF!="MVP","0.0 MVP",#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="S85" s="20" t="str">
+      <c r="S85" s="20">
         <f t="shared" si="5"/>
-        <v/>
+        <v>85</v>
       </c>
     </row>
     <row r="86" spans="1:19">
@@ -6158,19 +7670,29 @@
         <v/>
       </c>
     </row>
-    <row r="87" spans="1:19">
-      <c r="A87" s="9"/>
-      <c r="B87" s="10"/>
-      <c r="C87" s="11"/>
-      <c r="D87" s="12"/>
-      <c r="E87" s="13"/>
+    <row r="87" spans="1:19" ht="22.5">
+      <c r="A87" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="B87" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="C87" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D87" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E87" s="13" t="s">
+        <v>151</v>
+      </c>
       <c r="F87" s="13"/>
       <c r="G87" s="13"/>
       <c r="H87" s="13"/>
       <c r="I87" s="15"/>
-      <c r="J87" s="16" t="str">
+      <c r="J87" s="16">
         <f t="shared" si="3"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="K87" s="17" t="e">
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
@@ -6180,9 +7702,9 @@
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="M87" s="16" t="str">
+      <c r="M87" s="16">
         <f t="shared" si="4"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="N87" s="16" t="e">
         <f>IF(#REF!="1 High",4,IF(#REF!="2 Med",3,IF(#REF!="3 Med",2,IF(#REF!="4 Low",1,""))))</f>
@@ -6201,24 +7723,34 @@
         <f>IF(#REF!="MVP","0.0 MVP",#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="S87" s="20" t="str">
+      <c r="S87" s="20">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="88" spans="1:19">
-      <c r="A88" s="9"/>
-      <c r="B88" s="10"/>
-      <c r="C88" s="11"/>
-      <c r="D88" s="12"/>
-      <c r="E88" s="13"/>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="88" spans="1:19" ht="22.5">
+      <c r="A88" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="B88" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="C88" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D88" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E88" s="13" t="s">
+        <v>153</v>
+      </c>
       <c r="F88" s="13"/>
       <c r="G88" s="13"/>
       <c r="H88" s="13"/>
       <c r="I88" s="15"/>
-      <c r="J88" s="16" t="str">
+      <c r="J88" s="16">
         <f t="shared" si="3"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="K88" s="17" t="e">
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
@@ -6228,9 +7760,9 @@
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="M88" s="16" t="str">
+      <c r="M88" s="16">
         <f t="shared" si="4"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="N88" s="16" t="e">
         <f>IF(#REF!="1 High",4,IF(#REF!="2 Med",3,IF(#REF!="3 Med",2,IF(#REF!="4 Low",1,""))))</f>
@@ -6249,24 +7781,34 @@
         <f>IF(#REF!="MVP","0.0 MVP",#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="S88" s="20" t="str">
+      <c r="S88" s="20">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="89" spans="1:19">
-      <c r="A89" s="9"/>
-      <c r="B89" s="10"/>
-      <c r="C89" s="11"/>
-      <c r="D89" s="12"/>
-      <c r="E89" s="13"/>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="89" spans="1:19" ht="22.5">
+      <c r="A89" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="B89" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="C89" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D89" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E89" s="13" t="s">
+        <v>153</v>
+      </c>
       <c r="F89" s="13"/>
       <c r="G89" s="13"/>
       <c r="H89" s="13"/>
       <c r="I89" s="15"/>
-      <c r="J89" s="16" t="str">
+      <c r="J89" s="16">
         <f t="shared" si="3"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="K89" s="17" t="e">
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
@@ -6276,9 +7818,9 @@
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="M89" s="16" t="str">
+      <c r="M89" s="16">
         <f t="shared" si="4"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="N89" s="16" t="e">
         <f>IF(#REF!="1 High",4,IF(#REF!="2 Med",3,IF(#REF!="3 Med",2,IF(#REF!="4 Low",1,""))))</f>
@@ -6297,24 +7839,34 @@
         <f>IF(#REF!="MVP","0.0 MVP",#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="S89" s="20" t="str">
+      <c r="S89" s="20">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="90" spans="1:19">
-      <c r="A90" s="9"/>
-      <c r="B90" s="10"/>
-      <c r="C90" s="11"/>
-      <c r="D90" s="12"/>
-      <c r="E90" s="13"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="90" spans="1:19" ht="22.5">
+      <c r="A90" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="B90" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="C90" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D90" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E90" s="13" t="s">
+        <v>156</v>
+      </c>
       <c r="F90" s="13"/>
       <c r="G90" s="13"/>
       <c r="H90" s="13"/>
       <c r="I90" s="15"/>
-      <c r="J90" s="16" t="str">
+      <c r="J90" s="16">
         <f t="shared" si="3"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="K90" s="17" t="e">
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
@@ -6324,9 +7876,9 @@
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="M90" s="16" t="str">
+      <c r="M90" s="16">
         <f t="shared" si="4"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="N90" s="16" t="e">
         <f>IF(#REF!="1 High",4,IF(#REF!="2 Med",3,IF(#REF!="3 Med",2,IF(#REF!="4 Low",1,""))))</f>
@@ -6345,24 +7897,34 @@
         <f>IF(#REF!="MVP","0.0 MVP",#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="S90" s="20" t="str">
+      <c r="S90" s="20">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="91" spans="1:19">
-      <c r="A91" s="9"/>
-      <c r="B91" s="10"/>
-      <c r="C91" s="11"/>
-      <c r="D91" s="12"/>
-      <c r="E91" s="13"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="91" spans="1:19" ht="56.25">
+      <c r="A91" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="B91" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="C91" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D91" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E91" s="13" t="s">
+        <v>158</v>
+      </c>
       <c r="F91" s="13"/>
       <c r="G91" s="13"/>
       <c r="H91" s="13"/>
       <c r="I91" s="15"/>
-      <c r="J91" s="16" t="str">
+      <c r="J91" s="16">
         <f t="shared" si="3"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="K91" s="17" t="e">
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
@@ -6372,9 +7934,9 @@
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="M91" s="16" t="str">
+      <c r="M91" s="16">
         <f t="shared" si="4"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="N91" s="16" t="e">
         <f>IF(#REF!="1 High",4,IF(#REF!="2 Med",3,IF(#REF!="3 Med",2,IF(#REF!="4 Low",1,""))))</f>
@@ -6393,24 +7955,34 @@
         <f>IF(#REF!="MVP","0.0 MVP",#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="S91" s="20" t="str">
+      <c r="S91" s="20">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="92" spans="1:19">
-      <c r="A92" s="9"/>
-      <c r="B92" s="10"/>
-      <c r="C92" s="11"/>
-      <c r="D92" s="12"/>
-      <c r="E92" s="13"/>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="92" spans="1:19" ht="78.75">
+      <c r="A92" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="B92" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="C92" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D92" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E92" s="13" t="s">
+        <v>160</v>
+      </c>
       <c r="F92" s="13"/>
       <c r="G92" s="13"/>
       <c r="H92" s="13"/>
       <c r="I92" s="15"/>
-      <c r="J92" s="16" t="str">
+      <c r="J92" s="16">
         <f t="shared" si="3"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="K92" s="17" t="e">
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
@@ -6420,9 +7992,9 @@
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="M92" s="16" t="str">
+      <c r="M92" s="16">
         <f t="shared" si="4"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="N92" s="16" t="e">
         <f>IF(#REF!="1 High",4,IF(#REF!="2 Med",3,IF(#REF!="3 Med",2,IF(#REF!="4 Low",1,""))))</f>
@@ -6441,24 +8013,34 @@
         <f>IF(#REF!="MVP","0.0 MVP",#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="S92" s="20" t="str">
+      <c r="S92" s="20">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="93" spans="1:19">
-      <c r="A93" s="9"/>
-      <c r="B93" s="10"/>
-      <c r="C93" s="11"/>
-      <c r="D93" s="12"/>
-      <c r="E93" s="13"/>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="93" spans="1:19" ht="78.75">
+      <c r="A93" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="B93" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="C93" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D93" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E93" s="13" t="s">
+        <v>162</v>
+      </c>
       <c r="F93" s="13"/>
       <c r="G93" s="13"/>
       <c r="H93" s="13"/>
       <c r="I93" s="15"/>
-      <c r="J93" s="16" t="str">
+      <c r="J93" s="16">
         <f t="shared" si="3"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="K93" s="17" t="e">
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
@@ -6468,9 +8050,9 @@
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="M93" s="16" t="str">
+      <c r="M93" s="16">
         <f t="shared" si="4"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="N93" s="16" t="e">
         <f>IF(#REF!="1 High",4,IF(#REF!="2 Med",3,IF(#REF!="3 Med",2,IF(#REF!="4 Low",1,""))))</f>
@@ -6489,24 +8071,34 @@
         <f>IF(#REF!="MVP","0.0 MVP",#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="S93" s="20" t="str">
+      <c r="S93" s="20">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="94" spans="1:19">
-      <c r="A94" s="9"/>
-      <c r="B94" s="10"/>
-      <c r="C94" s="11"/>
-      <c r="D94" s="12"/>
-      <c r="E94" s="13"/>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="94" spans="1:19" ht="22.5">
+      <c r="A94" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="B94" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C94" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D94" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E94" s="13" t="s">
+        <v>164</v>
+      </c>
       <c r="F94" s="13"/>
       <c r="G94" s="13"/>
       <c r="H94" s="13"/>
       <c r="I94" s="15"/>
-      <c r="J94" s="16" t="str">
+      <c r="J94" s="16">
         <f t="shared" si="3"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="K94" s="17" t="e">
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
@@ -6516,9 +8108,9 @@
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="M94" s="16" t="str">
+      <c r="M94" s="16">
         <f t="shared" si="4"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="N94" s="16" t="e">
         <f>IF(#REF!="1 High",4,IF(#REF!="2 Med",3,IF(#REF!="3 Med",2,IF(#REF!="4 Low",1,""))))</f>
@@ -6537,24 +8129,34 @@
         <f>IF(#REF!="MVP","0.0 MVP",#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="S94" s="20" t="str">
+      <c r="S94" s="20">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="95" spans="1:19">
-      <c r="A95" s="9"/>
-      <c r="B95" s="10"/>
-      <c r="C95" s="11"/>
-      <c r="D95" s="12"/>
-      <c r="E95" s="13"/>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="95" spans="1:19" ht="56.25">
+      <c r="A95" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="B95" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="C95" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D95" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E95" s="13" t="s">
+        <v>166</v>
+      </c>
       <c r="F95" s="13"/>
       <c r="G95" s="13"/>
       <c r="H95" s="13"/>
       <c r="I95" s="15"/>
-      <c r="J95" s="16" t="str">
+      <c r="J95" s="16">
         <f t="shared" si="3"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="K95" s="17" t="e">
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
@@ -6564,9 +8166,9 @@
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="M95" s="16" t="str">
+      <c r="M95" s="16">
         <f t="shared" si="4"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="N95" s="16" t="e">
         <f>IF(#REF!="1 High",4,IF(#REF!="2 Med",3,IF(#REF!="3 Med",2,IF(#REF!="4 Low",1,""))))</f>
@@ -6585,24 +8187,34 @@
         <f>IF(#REF!="MVP","0.0 MVP",#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="S95" s="20" t="str">
+      <c r="S95" s="20">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="96" spans="1:19">
-      <c r="A96" s="9"/>
-      <c r="B96" s="10"/>
-      <c r="C96" s="11"/>
-      <c r="D96" s="12"/>
-      <c r="E96" s="13"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="96" spans="1:19" ht="78.75">
+      <c r="A96" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="B96" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="C96" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D96" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E96" s="13" t="s">
+        <v>162</v>
+      </c>
       <c r="F96" s="13"/>
       <c r="G96" s="13"/>
       <c r="H96" s="13"/>
       <c r="I96" s="15"/>
-      <c r="J96" s="16" t="str">
+      <c r="J96" s="16">
         <f t="shared" si="3"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="K96" s="17" t="e">
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
@@ -6612,9 +8224,9 @@
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="M96" s="16" t="str">
+      <c r="M96" s="16">
         <f t="shared" si="4"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="N96" s="16" t="e">
         <f>IF(#REF!="1 High",4,IF(#REF!="2 Med",3,IF(#REF!="3 Med",2,IF(#REF!="4 Low",1,""))))</f>
@@ -6633,24 +8245,34 @@
         <f>IF(#REF!="MVP","0.0 MVP",#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="S96" s="20" t="str">
+      <c r="S96" s="20">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="97" spans="1:19">
-      <c r="A97" s="9"/>
-      <c r="B97" s="10"/>
-      <c r="C97" s="11"/>
-      <c r="D97" s="12"/>
-      <c r="E97" s="13"/>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="97" spans="1:19" ht="101.25">
+      <c r="A97" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="B97" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="C97" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D97" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E97" s="13" t="s">
+        <v>169</v>
+      </c>
       <c r="F97" s="13"/>
       <c r="G97" s="13"/>
       <c r="H97" s="13"/>
       <c r="I97" s="15"/>
-      <c r="J97" s="16" t="str">
+      <c r="J97" s="16">
         <f t="shared" si="3"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="K97" s="17" t="e">
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
@@ -6660,9 +8282,9 @@
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="M97" s="16" t="str">
+      <c r="M97" s="16">
         <f t="shared" si="4"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="N97" s="16" t="e">
         <f>IF(#REF!="1 High",4,IF(#REF!="2 Med",3,IF(#REF!="3 Med",2,IF(#REF!="4 Low",1,""))))</f>
@@ -6681,9 +8303,9 @@
         <f>IF(#REF!="MVP","0.0 MVP",#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="S97" s="20" t="str">
+      <c r="S97" s="20">
         <f t="shared" si="5"/>
-        <v/>
+        <v>97</v>
       </c>
     </row>
     <row r="98" spans="1:19">
@@ -6782,19 +8404,29 @@
         <v/>
       </c>
     </row>
-    <row r="100" spans="1:19">
-      <c r="A100" s="9"/>
-      <c r="B100" s="10"/>
-      <c r="C100" s="11"/>
-      <c r="D100" s="12"/>
-      <c r="E100" s="13"/>
+    <row r="100" spans="1:19" ht="33.75">
+      <c r="A100" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="B100" s="10" t="s">
+        <v>171</v>
+      </c>
+      <c r="C100" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D100" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E100" s="13" t="s">
+        <v>172</v>
+      </c>
       <c r="F100" s="13"/>
       <c r="G100" s="13"/>
       <c r="H100" s="13"/>
       <c r="I100" s="15"/>
-      <c r="J100" s="16" t="str">
+      <c r="J100" s="16">
         <f t="shared" si="3"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="K100" s="17" t="e">
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
@@ -6804,9 +8436,9 @@
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="M100" s="16" t="str">
+      <c r="M100" s="16">
         <f t="shared" si="4"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="N100" s="16" t="e">
         <f>IF(#REF!="1 High",4,IF(#REF!="2 Med",3,IF(#REF!="3 Med",2,IF(#REF!="4 Low",1,""))))</f>
@@ -6825,17 +8457,19 @@
         <f>IF(#REF!="MVP","0.0 MVP",#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="S100" s="20" t="str">
+      <c r="S100" s="20">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="101" spans="1:19">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="101" spans="1:19" ht="22.5">
       <c r="A101" s="9"/>
       <c r="B101" s="10"/>
       <c r="C101" s="11"/>
       <c r="D101" s="12"/>
-      <c r="E101" s="13"/>
+      <c r="E101" s="13" t="s">
+        <v>173</v>
+      </c>
       <c r="F101" s="13"/>
       <c r="G101" s="13"/>
       <c r="H101" s="13"/>
@@ -7022,19 +8656,29 @@
         <v/>
       </c>
     </row>
-    <row r="105" spans="1:19">
-      <c r="A105" s="9"/>
-      <c r="B105" s="10"/>
-      <c r="C105" s="11"/>
-      <c r="D105" s="12"/>
-      <c r="E105" s="13"/>
+    <row r="105" spans="1:19" ht="33.75">
+      <c r="A105" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="B105" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="C105" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D105" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E105" s="13" t="s">
+        <v>175</v>
+      </c>
       <c r="F105" s="13"/>
       <c r="G105" s="13"/>
       <c r="H105" s="13"/>
       <c r="I105" s="15"/>
-      <c r="J105" s="16" t="str">
+      <c r="J105" s="16">
         <f t="shared" si="3"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="K105" s="17" t="e">
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
@@ -7044,9 +8688,9 @@
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="M105" s="16" t="str">
+      <c r="M105" s="16">
         <f t="shared" si="4"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="N105" s="16" t="e">
         <f>IF(#REF!="1 High",4,IF(#REF!="2 Med",3,IF(#REF!="3 Med",2,IF(#REF!="4 Low",1,""))))</f>
@@ -7065,17 +8709,19 @@
         <f>IF(#REF!="MVP","0.0 MVP",#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="S105" s="20" t="str">
+      <c r="S105" s="20">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="106" spans="1:19">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="106" spans="1:19" ht="33.75">
       <c r="A106" s="9"/>
       <c r="B106" s="10"/>
       <c r="C106" s="11"/>
       <c r="D106" s="12"/>
-      <c r="E106" s="13"/>
+      <c r="E106" s="13" t="s">
+        <v>176</v>
+      </c>
       <c r="F106" s="13"/>
       <c r="G106" s="13"/>
       <c r="H106" s="13"/>
@@ -7214,19 +8860,29 @@
         <v/>
       </c>
     </row>
-    <row r="109" spans="1:19">
-      <c r="A109" s="9"/>
-      <c r="B109" s="10"/>
-      <c r="C109" s="11"/>
-      <c r="D109" s="12"/>
-      <c r="E109" s="13"/>
+    <row r="109" spans="1:19" ht="22.5">
+      <c r="A109" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="B109" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="C109" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D109" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E109" s="13" t="s">
+        <v>178</v>
+      </c>
       <c r="F109" s="13"/>
       <c r="G109" s="13"/>
       <c r="H109" s="13"/>
       <c r="I109" s="15"/>
-      <c r="J109" s="16" t="str">
+      <c r="J109" s="16">
         <f t="shared" si="3"/>
-        <v/>
+        <v>1</v>
       </c>
       <c r="K109" s="17" t="e">
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
@@ -7236,9 +8892,9 @@
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="M109" s="16" t="str">
+      <c r="M109" s="16">
         <f t="shared" si="4"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="N109" s="16" t="e">
         <f>IF(#REF!="1 High",4,IF(#REF!="2 Med",3,IF(#REF!="3 Med",2,IF(#REF!="4 Low",1,""))))</f>
@@ -7257,24 +8913,34 @@
         <f>IF(#REF!="MVP","0.0 MVP",#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="S109" s="20" t="str">
+      <c r="S109" s="20">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="110" spans="1:19">
-      <c r="A110" s="9"/>
-      <c r="B110" s="10"/>
-      <c r="C110" s="11"/>
-      <c r="D110" s="12"/>
-      <c r="E110" s="13"/>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="110" spans="1:19" ht="22.5">
+      <c r="A110" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="B110" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="C110" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D110" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E110" s="13" t="s">
+        <v>180</v>
+      </c>
       <c r="F110" s="13"/>
       <c r="G110" s="13"/>
       <c r="H110" s="13"/>
       <c r="I110" s="15"/>
-      <c r="J110" s="16" t="str">
+      <c r="J110" s="16">
         <f t="shared" si="3"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="K110" s="17" t="e">
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
@@ -7284,9 +8950,9 @@
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="M110" s="16" t="str">
+      <c r="M110" s="16">
         <f t="shared" si="4"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="N110" s="16" t="e">
         <f>IF(#REF!="1 High",4,IF(#REF!="2 Med",3,IF(#REF!="3 Med",2,IF(#REF!="4 Low",1,""))))</f>
@@ -7305,24 +8971,34 @@
         <f>IF(#REF!="MVP","0.0 MVP",#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="S110" s="20" t="str">
+      <c r="S110" s="20">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="111" spans="1:19">
-      <c r="A111" s="9"/>
-      <c r="B111" s="10"/>
-      <c r="C111" s="11"/>
-      <c r="D111" s="12"/>
-      <c r="E111" s="13"/>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="111" spans="1:19" ht="22.5">
+      <c r="A111" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="B111" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="C111" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D111" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E111" s="13" t="s">
+        <v>182</v>
+      </c>
       <c r="F111" s="13"/>
       <c r="G111" s="13"/>
       <c r="H111" s="13"/>
       <c r="I111" s="15"/>
-      <c r="J111" s="16" t="str">
+      <c r="J111" s="16">
         <f t="shared" si="3"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="K111" s="17" t="e">
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
@@ -7332,9 +9008,9 @@
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="M111" s="16" t="str">
+      <c r="M111" s="16">
         <f t="shared" si="4"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="N111" s="16" t="e">
         <f>IF(#REF!="1 High",4,IF(#REF!="2 Med",3,IF(#REF!="3 Med",2,IF(#REF!="4 Low",1,""))))</f>
@@ -7353,24 +9029,34 @@
         <f>IF(#REF!="MVP","0.0 MVP",#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="S111" s="20" t="str">
+      <c r="S111" s="20">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="112" spans="1:19">
-      <c r="A112" s="9"/>
-      <c r="B112" s="10"/>
-      <c r="C112" s="11"/>
-      <c r="D112" s="12"/>
-      <c r="E112" s="13"/>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="112" spans="1:19" ht="33.75">
+      <c r="A112" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="B112" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="C112" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D112" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E112" s="13" t="s">
+        <v>184</v>
+      </c>
       <c r="F112" s="13"/>
       <c r="G112" s="13"/>
       <c r="H112" s="13"/>
       <c r="I112" s="15"/>
-      <c r="J112" s="16" t="str">
+      <c r="J112" s="16">
         <f t="shared" si="3"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="K112" s="17" t="e">
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
@@ -7380,9 +9066,9 @@
         <f>IF(#REF!="1 High",1,IF(#REF!="2 Med",2,IF(#REF!="3 Med",3,IF(#REF!="4 Low",4,""))))</f>
         <v>#REF!</v>
       </c>
-      <c r="M112" s="16" t="str">
+      <c r="M112" s="16">
         <f t="shared" si="4"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="N112" s="16" t="e">
         <f>IF(#REF!="1 High",4,IF(#REF!="2 Med",3,IF(#REF!="3 Med",2,IF(#REF!="4 Low",1,""))))</f>
@@ -7401,9 +9087,9 @@
         <f>IF(#REF!="MVP","0.0 MVP",#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="S112" s="20" t="str">
+      <c r="S112" s="20">
         <f t="shared" si="5"/>
-        <v/>
+        <v>112</v>
       </c>
     </row>
     <row r="113" spans="1:19">
@@ -52476,242 +54162,571 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C31 C52:C1000">
-    <cfRule type="containsText" dxfId="45" priority="25" operator="containsText" text="1"/>
+  <conditionalFormatting sqref="C1:C31 C52:C83 C86 C113:C1000">
+    <cfRule type="containsText" dxfId="183" priority="94" operator="containsText" text="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C31 C52:C1000">
-    <cfRule type="containsText" dxfId="44" priority="26" operator="containsText" text="2"/>
+  <conditionalFormatting sqref="C1:C31 C52:C83 C86 C113:C1000">
+    <cfRule type="containsText" dxfId="182" priority="95" operator="containsText" text="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C31 C52:C1000">
-    <cfRule type="containsText" dxfId="43" priority="27" operator="containsText" text="3"/>
+  <conditionalFormatting sqref="C1:C31 C52:C83 C86 C113:C1000">
+    <cfRule type="containsText" dxfId="181" priority="96" operator="containsText" text="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C31 C52:C1000">
-    <cfRule type="containsText" dxfId="42" priority="28" operator="containsText" text="4"/>
+  <conditionalFormatting sqref="C1:C31 C52:C83 C86 C113:C1000">
+    <cfRule type="containsText" dxfId="180" priority="97" operator="containsText" text="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D31 D52:D1000">
-    <cfRule type="cellIs" dxfId="41" priority="29" operator="equal">
+  <conditionalFormatting sqref="D2:D31 D52:D83 D86 D113:D1000">
+    <cfRule type="cellIs" dxfId="179" priority="98" operator="equal">
       <formula>"?"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D31 D52:D1000">
-    <cfRule type="cellIs" dxfId="40" priority="30" operator="equal">
+  <conditionalFormatting sqref="D2:D31 D52:D83 D86 D113:D1000">
+    <cfRule type="cellIs" dxfId="178" priority="99" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D31 D52:D1000">
-    <cfRule type="cellIs" dxfId="39" priority="31" operator="equal">
+  <conditionalFormatting sqref="D2:D31 D52:D83 D86 D113:D1000">
+    <cfRule type="cellIs" dxfId="177" priority="100" operator="equal">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D31 D52:D1000">
-    <cfRule type="cellIs" dxfId="38" priority="32" operator="equal">
+  <conditionalFormatting sqref="D2:D31 D52:D83 D86 D113:D1000">
+    <cfRule type="cellIs" dxfId="176" priority="101" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D31 D52:D1000">
-    <cfRule type="cellIs" dxfId="37" priority="33" operator="equal">
+  <conditionalFormatting sqref="D2:D31 D52:D83 D86 D113:D1000">
+    <cfRule type="cellIs" dxfId="175" priority="102" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D31 D52:D1000">
-    <cfRule type="cellIs" dxfId="36" priority="34" operator="equal">
+  <conditionalFormatting sqref="D2:D31 D52:D83 D86 D113:D1000">
+    <cfRule type="cellIs" dxfId="174" priority="103" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D31 D52:D1000">
-    <cfRule type="cellIs" dxfId="35" priority="35" operator="equal">
+  <conditionalFormatting sqref="D2:D31 D52:D83 D86 D113:D1000">
+    <cfRule type="cellIs" dxfId="173" priority="104" operator="equal">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D31 D52:D1000">
-    <cfRule type="cellIs" dxfId="34" priority="36" operator="equal">
+  <conditionalFormatting sqref="D2:D31 D52:D83 D86 D113:D1000">
+    <cfRule type="cellIs" dxfId="172" priority="105" operator="equal">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D31 D52:D1000">
-    <cfRule type="cellIs" dxfId="33" priority="37" operator="equal">
+  <conditionalFormatting sqref="D2:D31 D52:D83 D86 D113:D1000">
+    <cfRule type="cellIs" dxfId="171" priority="106" operator="equal">
       <formula>13</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D31 D52:D1000">
-    <cfRule type="cellIs" dxfId="32" priority="38" operator="equal">
+  <conditionalFormatting sqref="D2:D31 D52:D83 D86 D113:D1000">
+    <cfRule type="cellIs" dxfId="170" priority="107" operator="equal">
       <formula>21</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D31 D52:D1000">
-    <cfRule type="cellIs" dxfId="31" priority="39" operator="equal">
+  <conditionalFormatting sqref="D2:D31 D52:D83 D86 D113:D1000">
+    <cfRule type="cellIs" dxfId="169" priority="108" operator="equal">
       <formula>34</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D31 D52:D1000">
-    <cfRule type="cellIs" dxfId="30" priority="40" operator="equal">
+  <conditionalFormatting sqref="D2:D31 D52:D83 D86 D113:D1000">
+    <cfRule type="cellIs" dxfId="168" priority="109" operator="equal">
       <formula>55</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D31 D52:D1000">
-    <cfRule type="cellIs" dxfId="29" priority="41" operator="equal">
+  <conditionalFormatting sqref="D2:D31 D52:D83 D86 D113:D1000">
+    <cfRule type="cellIs" dxfId="167" priority="110" operator="equal">
       <formula>89</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D31 D52:D1000">
-    <cfRule type="cellIs" dxfId="28" priority="42" operator="equal">
+  <conditionalFormatting sqref="D2:D31 D52:D83 D86 D113:D1000">
+    <cfRule type="cellIs" dxfId="166" priority="111" operator="equal">
       <formula>"XSM"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D31 D52:D1000">
-    <cfRule type="cellIs" dxfId="27" priority="43" operator="equal">
+  <conditionalFormatting sqref="D2:D31 D52:D83 D86 D113:D1000">
+    <cfRule type="cellIs" dxfId="165" priority="112" operator="equal">
       <formula>"SM"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D31 D52:D1000">
-    <cfRule type="cellIs" dxfId="26" priority="44" operator="equal">
+  <conditionalFormatting sqref="D2:D31 D52:D83 D86 D113:D1000">
+    <cfRule type="cellIs" dxfId="164" priority="113" operator="equal">
       <formula>"MD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D31 D52:D1000">
-    <cfRule type="cellIs" dxfId="25" priority="45" operator="equal">
+  <conditionalFormatting sqref="D2:D31 D52:D83 D86 D113:D1000">
+    <cfRule type="cellIs" dxfId="163" priority="114" operator="equal">
       <formula>"LG"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D31 D52:D1000">
-    <cfRule type="cellIs" dxfId="24" priority="46" operator="equal">
+  <conditionalFormatting sqref="D2:D31 D52:D83 D86 D113:D1000">
+    <cfRule type="cellIs" dxfId="162" priority="115" operator="equal">
       <formula>"XLG"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D31 D52:D1000">
-    <cfRule type="cellIs" dxfId="23" priority="47" operator="equal">
+  <conditionalFormatting sqref="D2:D31 D52:D83 D86 D113:D1000">
+    <cfRule type="cellIs" dxfId="161" priority="116" operator="equal">
       <formula>"XXLG"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32:C51">
-    <cfRule type="containsText" dxfId="22" priority="1" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="160" priority="70" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH(("1"),(C32))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32:C51">
-    <cfRule type="containsText" dxfId="21" priority="2" operator="containsText" text="2">
+    <cfRule type="containsText" dxfId="159" priority="71" operator="containsText" text="2">
       <formula>NOT(ISERROR(SEARCH(("2"),(C32))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32:C51">
-    <cfRule type="containsText" dxfId="20" priority="3" operator="containsText" text="3">
+    <cfRule type="containsText" dxfId="158" priority="72" operator="containsText" text="3">
       <formula>NOT(ISERROR(SEARCH(("3"),(C32))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32:C51">
-    <cfRule type="containsText" dxfId="19" priority="4" operator="containsText" text="4">
+    <cfRule type="containsText" dxfId="157" priority="73" operator="containsText" text="4">
       <formula>NOT(ISERROR(SEARCH(("4"),(C32))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32:D51">
-    <cfRule type="cellIs" dxfId="18" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="156" priority="74" operator="equal">
       <formula>"?"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32:D51">
-    <cfRule type="cellIs" dxfId="17" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="75" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32:D51">
-    <cfRule type="cellIs" dxfId="16" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="76" operator="equal">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32:D51">
-    <cfRule type="cellIs" dxfId="15" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="77" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32:D51">
-    <cfRule type="cellIs" dxfId="14" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="78" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32:D51">
-    <cfRule type="cellIs" dxfId="13" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="79" operator="equal">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32:D51">
-    <cfRule type="cellIs" dxfId="12" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="80" operator="equal">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32:D51">
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="81" operator="equal">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32:D51">
-    <cfRule type="cellIs" dxfId="10" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="148" priority="82" operator="equal">
       <formula>13</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32:D51">
-    <cfRule type="cellIs" dxfId="9" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="83" operator="equal">
       <formula>21</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32:D51">
-    <cfRule type="cellIs" dxfId="8" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="84" operator="equal">
       <formula>34</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32:D51">
-    <cfRule type="cellIs" dxfId="7" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="85" operator="equal">
       <formula>55</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32:D51">
-    <cfRule type="cellIs" dxfId="6" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="86" operator="equal">
       <formula>89</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32:D51">
-    <cfRule type="cellIs" dxfId="5" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="87" operator="equal">
       <formula>"XSM"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32:D51">
-    <cfRule type="cellIs" dxfId="4" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="88" operator="equal">
       <formula>"SM"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32:D51">
-    <cfRule type="cellIs" dxfId="3" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="89" operator="equal">
       <formula>"MD"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32:D51">
-    <cfRule type="cellIs" dxfId="2" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="90" operator="equal">
       <formula>"LG"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32:D51">
-    <cfRule type="cellIs" dxfId="1" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="91" operator="equal">
       <formula>"XLG"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32:D51">
-    <cfRule type="cellIs" dxfId="0" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="92" operator="equal">
       <formula>"XXLG"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" sqref="C2:C31 C52:C1000" xr:uid="{00000000-0002-0000-0000-000000000000}">
+  <conditionalFormatting sqref="C84:C85">
+    <cfRule type="containsText" dxfId="137" priority="47" operator="containsText" text="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C84:C85">
+    <cfRule type="containsText" dxfId="135" priority="48" operator="containsText" text="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C84:C85">
+    <cfRule type="containsText" dxfId="133" priority="49" operator="containsText" text="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C84:C85">
+    <cfRule type="containsText" dxfId="131" priority="50" operator="containsText" text="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D84:D85">
+    <cfRule type="cellIs" dxfId="129" priority="51" operator="equal">
+      <formula>"?"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D84:D85">
+    <cfRule type="cellIs" dxfId="127" priority="52" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D84:D85">
+    <cfRule type="cellIs" dxfId="125" priority="53" operator="equal">
+      <formula>0.5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D84:D85">
+    <cfRule type="cellIs" dxfId="123" priority="54" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D84:D85">
+    <cfRule type="cellIs" dxfId="121" priority="55" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D84:D85">
+    <cfRule type="cellIs" dxfId="119" priority="56" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D84:D85">
+    <cfRule type="cellIs" dxfId="117" priority="57" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D84:D85">
+    <cfRule type="cellIs" dxfId="115" priority="58" operator="equal">
+      <formula>8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D84:D85">
+    <cfRule type="cellIs" dxfId="113" priority="59" operator="equal">
+      <formula>13</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D84:D85">
+    <cfRule type="cellIs" dxfId="111" priority="60" operator="equal">
+      <formula>21</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D84:D85">
+    <cfRule type="cellIs" dxfId="109" priority="61" operator="equal">
+      <formula>34</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D84:D85">
+    <cfRule type="cellIs" dxfId="107" priority="62" operator="equal">
+      <formula>55</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D84:D85">
+    <cfRule type="cellIs" dxfId="105" priority="63" operator="equal">
+      <formula>89</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D84:D85">
+    <cfRule type="cellIs" dxfId="103" priority="64" operator="equal">
+      <formula>"XSM"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D84:D85">
+    <cfRule type="cellIs" dxfId="101" priority="65" operator="equal">
+      <formula>"SM"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D84:D85">
+    <cfRule type="cellIs" dxfId="99" priority="66" operator="equal">
+      <formula>"MD"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D84:D85">
+    <cfRule type="cellIs" dxfId="97" priority="67" operator="equal">
+      <formula>"LG"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D84:D85">
+    <cfRule type="cellIs" dxfId="95" priority="68" operator="equal">
+      <formula>"XLG"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D84:D85">
+    <cfRule type="cellIs" dxfId="93" priority="69" operator="equal">
+      <formula>"XXLG"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C87:C99 C109">
+    <cfRule type="containsText" dxfId="91" priority="1" operator="containsText" text="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C87:C99 C109">
+    <cfRule type="containsText" dxfId="89" priority="2" operator="containsText" text="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C87:C99 C109">
+    <cfRule type="containsText" dxfId="87" priority="3" operator="containsText" text="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C87:C99 C109">
+    <cfRule type="containsText" dxfId="85" priority="4" operator="containsText" text="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D87:D99">
+    <cfRule type="cellIs" dxfId="83" priority="5" operator="equal">
+      <formula>"?"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D87:D99">
+    <cfRule type="cellIs" dxfId="81" priority="6" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D87:D99">
+    <cfRule type="cellIs" dxfId="79" priority="7" operator="equal">
+      <formula>0.5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D87:D99">
+    <cfRule type="cellIs" dxfId="77" priority="8" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D87:D99">
+    <cfRule type="cellIs" dxfId="75" priority="9" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D87:D99">
+    <cfRule type="cellIs" dxfId="73" priority="10" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D87:D99">
+    <cfRule type="cellIs" dxfId="71" priority="11" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D87:D99">
+    <cfRule type="cellIs" dxfId="69" priority="12" operator="equal">
+      <formula>8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D87:D99">
+    <cfRule type="cellIs" dxfId="67" priority="13" operator="equal">
+      <formula>13</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D87:D99">
+    <cfRule type="cellIs" dxfId="65" priority="14" operator="equal">
+      <formula>21</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D87:D99">
+    <cfRule type="cellIs" dxfId="63" priority="15" operator="equal">
+      <formula>34</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D87:D99">
+    <cfRule type="cellIs" dxfId="61" priority="16" operator="equal">
+      <formula>55</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D87:D99">
+    <cfRule type="cellIs" dxfId="59" priority="17" operator="equal">
+      <formula>89</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D87:D99">
+    <cfRule type="cellIs" dxfId="57" priority="18" operator="equal">
+      <formula>"XSM"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D87:D99">
+    <cfRule type="cellIs" dxfId="55" priority="19" operator="equal">
+      <formula>"SM"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D87:D99">
+    <cfRule type="cellIs" dxfId="53" priority="20" operator="equal">
+      <formula>"MD"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D87:D99">
+    <cfRule type="cellIs" dxfId="51" priority="21" operator="equal">
+      <formula>"LG"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D87:D99">
+    <cfRule type="cellIs" dxfId="49" priority="22" operator="equal">
+      <formula>"XLG"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D87:D99">
+    <cfRule type="cellIs" dxfId="47" priority="23" operator="equal">
+      <formula>"XXLG"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C100:C108 C110:C112">
+    <cfRule type="containsText" dxfId="45" priority="24" operator="containsText" text="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C100:C108 C110:C112">
+    <cfRule type="containsText" dxfId="43" priority="25" operator="containsText" text="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C100:C108 C110:C112">
+    <cfRule type="containsText" dxfId="41" priority="26" operator="containsText" text="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C100:C108 C110:C112">
+    <cfRule type="containsText" dxfId="39" priority="27" operator="containsText" text="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D100:D112">
+    <cfRule type="cellIs" dxfId="37" priority="28" operator="equal">
+      <formula>"?"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D100:D112">
+    <cfRule type="cellIs" dxfId="35" priority="29" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D100:D112">
+    <cfRule type="cellIs" dxfId="33" priority="30" operator="equal">
+      <formula>0.5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D100:D112">
+    <cfRule type="cellIs" dxfId="31" priority="31" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D100:D112">
+    <cfRule type="cellIs" dxfId="29" priority="32" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D100:D112">
+    <cfRule type="cellIs" dxfId="27" priority="33" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D100:D112">
+    <cfRule type="cellIs" dxfId="25" priority="34" operator="equal">
+      <formula>5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D100:D112">
+    <cfRule type="cellIs" dxfId="23" priority="35" operator="equal">
+      <formula>8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D100:D112">
+    <cfRule type="cellIs" dxfId="21" priority="36" operator="equal">
+      <formula>13</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D100:D112">
+    <cfRule type="cellIs" dxfId="19" priority="37" operator="equal">
+      <formula>21</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D100:D112">
+    <cfRule type="cellIs" dxfId="17" priority="38" operator="equal">
+      <formula>34</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D100:D112">
+    <cfRule type="cellIs" dxfId="15" priority="39" operator="equal">
+      <formula>55</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D100:D112">
+    <cfRule type="cellIs" dxfId="13" priority="40" operator="equal">
+      <formula>89</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D100:D112">
+    <cfRule type="cellIs" dxfId="11" priority="41" operator="equal">
+      <formula>"XSM"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D100:D112">
+    <cfRule type="cellIs" dxfId="9" priority="42" operator="equal">
+      <formula>"SM"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D100:D112">
+    <cfRule type="cellIs" dxfId="7" priority="43" operator="equal">
+      <formula>"MD"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D100:D112">
+    <cfRule type="cellIs" dxfId="5" priority="44" operator="equal">
+      <formula>"LG"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D100:D112">
+    <cfRule type="cellIs" dxfId="3" priority="45" operator="equal">
+      <formula>"XLG"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D100:D112">
+    <cfRule type="cellIs" dxfId="1" priority="46" operator="equal">
+      <formula>"XXLG"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="6">
+    <dataValidation type="list" allowBlank="1" sqref="C2:C31 C52:C99 C113:C1000 C109">
       <formula1>"1 High,2 Med,3 Med,4 Low"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D2:D31 D52:D1000" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" sqref="D2:D31 D52:D99 D113:D1000">
       <formula1>"XSM,SM,MD,LG,XLG,XXLG,0,0.5,1,2,3,5,8,13,21,34,55,89,?"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D32:D51" xr:uid="{A40094A3-AD05-4DE3-BAC8-EF421913345A}">
+    <dataValidation type="list" allowBlank="1" sqref="D32:D51">
       <formula1>"XSM,SM,MD,LG,XLG,XXLG,0,0.5,1,2,3,5,8,13,21,34,55,89,?"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="C32:C51" xr:uid="{48DFC084-06CD-47C2-AAA7-50B9A3006CA2}">
+    <dataValidation type="list" allowBlank="1" sqref="C32:C51">
       <formula1>"1 High,2 Med,3 Med,4 Low"</formula1>
+    </dataValidation>
+    <dataValidation type="list" operator="equal" allowBlank="1" sqref="D100:D112">
+      <formula1>"XSM,SM,MD,LG,XLG,XXLG,0,0.5,1,2,3,5,8,13,21,34,55,89,?"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation type="list" operator="equal" allowBlank="1" sqref="C100:C108 C110:C112">
+      <formula1>"1 High,2 Med,3 Med,4 Low"</formula1>
+      <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -52720,7 +54735,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFA64D79"/>
   </sheetPr>

</xml_diff>